<commit_message>
Add features for 20k@20%
</commit_message>
<xml_diff>
--- a/results/features.xlsx
+++ b/results/features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\git\TCC-80true20fake\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6E7AD4-5BA6-4199-85C8-99CA55F5F19A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E960FC4-0463-44FD-9572-D7A3D4783394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{AA1E0EFD-90E7-4043-8413-F3444E557211}"/>
   </bookViews>
@@ -2556,6 +2556,603 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-5BBD-4578-9A57-8099D05C0EC9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$A$2:$A$92</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$F$2:$F$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>69913</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1153</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>873</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>702</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>393</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A90-4641-9152-5B49D48249F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3315,16 +3912,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3652,7 +4249,7 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3673,6 +4270,9 @@
       <c r="E1" s="1">
         <v>10000</v>
       </c>
+      <c r="F1" s="1">
+        <v>20000</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -3690,7 +4290,9 @@
       <c r="E2" s="1">
         <v>50529</v>
       </c>
-      <c r="F2"/>
+      <c r="F2" s="1">
+        <v>69913</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -3708,7 +4310,9 @@
       <c r="E3" s="1">
         <v>2680</v>
       </c>
-      <c r="F3"/>
+      <c r="F3" s="1">
+        <v>2679</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -3726,7 +4330,9 @@
       <c r="E4" s="1">
         <v>1625</v>
       </c>
-      <c r="F4"/>
+      <c r="F4" s="1">
+        <v>1614</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -3744,7 +4350,9 @@
       <c r="E5" s="1">
         <v>1152</v>
       </c>
-      <c r="F5"/>
+      <c r="F5" s="1">
+        <v>1153</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -3762,7 +4370,9 @@
       <c r="E6" s="1">
         <v>873</v>
       </c>
-      <c r="F6"/>
+      <c r="F6" s="1">
+        <v>873</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -3780,7 +4390,9 @@
       <c r="E7" s="1">
         <v>698</v>
       </c>
-      <c r="F7"/>
+      <c r="F7" s="1">
+        <v>702</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -3798,7 +4410,9 @@
       <c r="E8" s="1">
         <v>582</v>
       </c>
-      <c r="F8"/>
+      <c r="F8" s="1">
+        <v>584</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -3816,7 +4430,9 @@
       <c r="E9" s="1">
         <v>471</v>
       </c>
-      <c r="F9"/>
+      <c r="F9" s="1">
+        <v>475</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -3834,7 +4450,9 @@
       <c r="E10" s="1">
         <v>394</v>
       </c>
-      <c r="F10"/>
+      <c r="F10" s="1">
+        <v>393</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -3852,7 +4470,9 @@
       <c r="E11" s="1">
         <v>333</v>
       </c>
-      <c r="F11"/>
+      <c r="F11" s="1">
+        <v>330</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -3870,7 +4490,9 @@
       <c r="E12" s="1">
         <v>277</v>
       </c>
-      <c r="F12"/>
+      <c r="F12" s="1">
+        <v>276</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -3888,7 +4510,9 @@
       <c r="E13" s="1">
         <v>247</v>
       </c>
-      <c r="F13"/>
+      <c r="F13" s="1">
+        <v>248</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -3906,7 +4530,9 @@
       <c r="E14" s="1">
         <v>208</v>
       </c>
-      <c r="F14"/>
+      <c r="F14" s="1">
+        <v>208</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -3924,7 +4550,9 @@
       <c r="E15" s="1">
         <v>186</v>
       </c>
-      <c r="F15"/>
+      <c r="F15" s="1">
+        <v>186</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -3942,7 +4570,9 @@
       <c r="E16" s="1">
         <v>156</v>
       </c>
-      <c r="F16"/>
+      <c r="F16" s="1">
+        <v>153</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -3960,7 +4590,9 @@
       <c r="E17" s="1">
         <v>139</v>
       </c>
-      <c r="F17"/>
+      <c r="F17" s="1">
+        <v>138</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -3978,7 +4610,9 @@
       <c r="E18" s="1">
         <v>120</v>
       </c>
-      <c r="F18"/>
+      <c r="F18" s="1">
+        <v>119</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -3996,7 +4630,9 @@
       <c r="E19" s="1">
         <v>107</v>
       </c>
-      <c r="F19"/>
+      <c r="F19" s="1">
+        <v>107</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4014,7 +4650,9 @@
       <c r="E20" s="1">
         <v>98</v>
       </c>
-      <c r="F20"/>
+      <c r="F20" s="1">
+        <v>97</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -4032,7 +4670,9 @@
       <c r="E21" s="1">
         <v>90</v>
       </c>
-      <c r="F21"/>
+      <c r="F21" s="1">
+        <v>90</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -4050,7 +4690,9 @@
       <c r="E22" s="1">
         <v>82</v>
       </c>
-      <c r="F22"/>
+      <c r="F22" s="1">
+        <v>81</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -4068,7 +4710,9 @@
       <c r="E23" s="1">
         <v>76</v>
       </c>
-      <c r="F23"/>
+      <c r="F23" s="1">
+        <v>74</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -4086,7 +4730,9 @@
       <c r="E24" s="1">
         <v>67</v>
       </c>
-      <c r="F24"/>
+      <c r="F24" s="1">
+        <v>64</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -4104,7 +4750,9 @@
       <c r="E25" s="1">
         <v>56</v>
       </c>
-      <c r="F25"/>
+      <c r="F25" s="1">
+        <v>55</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -4122,7 +4770,9 @@
       <c r="E26" s="1">
         <v>49</v>
       </c>
-      <c r="F26"/>
+      <c r="F26" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -4140,7 +4790,9 @@
       <c r="E27" s="1">
         <v>42</v>
       </c>
-      <c r="F27"/>
+      <c r="F27" s="1">
+        <v>42</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -4158,7 +4810,9 @@
       <c r="E28" s="1">
         <v>37</v>
       </c>
-      <c r="F28"/>
+      <c r="F28" s="1">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -4176,7 +4830,9 @@
       <c r="E29" s="1">
         <v>32</v>
       </c>
-      <c r="F29"/>
+      <c r="F29" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -4194,7 +4850,9 @@
       <c r="E30" s="1">
         <v>29</v>
       </c>
-      <c r="F30"/>
+      <c r="F30" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -4212,7 +4870,9 @@
       <c r="E31" s="1">
         <v>27</v>
       </c>
-      <c r="F31"/>
+      <c r="F31" s="1">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
@@ -4230,7 +4890,9 @@
       <c r="E32" s="1">
         <v>26</v>
       </c>
-      <c r="F32"/>
+      <c r="F32" s="1">
+        <v>26</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
@@ -4248,7 +4910,9 @@
       <c r="E33" s="1">
         <v>26</v>
       </c>
-      <c r="F33"/>
+      <c r="F33" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -4266,7 +4930,9 @@
       <c r="E34" s="1">
         <v>24</v>
       </c>
-      <c r="F34"/>
+      <c r="F34" s="1">
+        <v>24</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
@@ -4284,7 +4950,9 @@
       <c r="E35" s="1">
         <v>22</v>
       </c>
-      <c r="F35"/>
+      <c r="F35" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -4302,7 +4970,9 @@
       <c r="E36" s="1">
         <v>22</v>
       </c>
-      <c r="F36"/>
+      <c r="F36" s="1">
+        <v>21</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -4320,7 +4990,9 @@
       <c r="E37" s="1">
         <v>20</v>
       </c>
-      <c r="F37"/>
+      <c r="F37" s="1">
+        <v>19</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
@@ -4338,7 +5010,9 @@
       <c r="E38" s="1">
         <v>17</v>
       </c>
-      <c r="F38"/>
+      <c r="F38" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
@@ -4356,7 +5030,9 @@
       <c r="E39" s="1">
         <v>16</v>
       </c>
-      <c r="F39"/>
+      <c r="F39" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
@@ -4374,7 +5050,9 @@
       <c r="E40" s="1">
         <v>14</v>
       </c>
-      <c r="F40"/>
+      <c r="F40" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -4392,7 +5070,9 @@
       <c r="E41" s="1">
         <v>13</v>
       </c>
-      <c r="F41"/>
+      <c r="F41" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -4410,7 +5090,9 @@
       <c r="E42" s="1">
         <v>12</v>
       </c>
-      <c r="F42"/>
+      <c r="F42" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
@@ -4428,7 +5110,9 @@
       <c r="E43" s="1">
         <v>11</v>
       </c>
-      <c r="F43"/>
+      <c r="F43" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -4446,7 +5130,9 @@
       <c r="E44" s="1">
         <v>10</v>
       </c>
-      <c r="F44"/>
+      <c r="F44" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
@@ -4464,7 +5150,9 @@
       <c r="E45" s="1">
         <v>8</v>
       </c>
-      <c r="F45"/>
+      <c r="F45" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
@@ -4482,7 +5170,9 @@
       <c r="E46" s="1">
         <v>7</v>
       </c>
-      <c r="F46"/>
+      <c r="F46" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
@@ -4500,7 +5190,9 @@
       <c r="E47" s="1">
         <v>5</v>
       </c>
-      <c r="F47"/>
+      <c r="F47" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -4518,7 +5210,9 @@
       <c r="E48" s="1">
         <v>5</v>
       </c>
-      <c r="F48"/>
+      <c r="F48" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -4536,7 +5230,9 @@
       <c r="E49" s="1">
         <v>5</v>
       </c>
-      <c r="F49"/>
+      <c r="F49" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
@@ -4554,7 +5250,9 @@
       <c r="E50" s="1">
         <v>4</v>
       </c>
-      <c r="F50"/>
+      <c r="F50" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -4572,7 +5270,9 @@
       <c r="E51" s="1">
         <v>4</v>
       </c>
-      <c r="F51"/>
+      <c r="F51" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
@@ -4590,7 +5290,9 @@
       <c r="E52" s="1">
         <v>4</v>
       </c>
-      <c r="F52"/>
+      <c r="F52" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
@@ -4608,7 +5310,9 @@
       <c r="E53" s="1">
         <v>4</v>
       </c>
-      <c r="F53"/>
+      <c r="F53" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
@@ -4626,7 +5330,9 @@
       <c r="E54" s="1">
         <v>4</v>
       </c>
-      <c r="F54"/>
+      <c r="F54" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -4644,7 +5350,9 @@
       <c r="E55" s="1">
         <v>4</v>
       </c>
-      <c r="F55"/>
+      <c r="F55" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
@@ -4662,7 +5370,9 @@
       <c r="E56" s="1">
         <v>3</v>
       </c>
-      <c r="F56"/>
+      <c r="F56" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
@@ -4680,7 +5390,9 @@
       <c r="E57" s="1">
         <v>3</v>
       </c>
-      <c r="F57"/>
+      <c r="F57" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
@@ -4698,7 +5410,9 @@
       <c r="E58" s="1">
         <v>3</v>
       </c>
-      <c r="F58"/>
+      <c r="F58" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
@@ -4716,7 +5430,9 @@
       <c r="E59" s="1">
         <v>3</v>
       </c>
-      <c r="F59"/>
+      <c r="F59" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
@@ -4734,7 +5450,9 @@
       <c r="E60" s="1">
         <v>3</v>
       </c>
-      <c r="F60"/>
+      <c r="F60" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
@@ -4752,7 +5470,9 @@
       <c r="E61" s="1">
         <v>2</v>
       </c>
-      <c r="F61"/>
+      <c r="F61" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
@@ -4770,7 +5490,9 @@
       <c r="E62" s="1">
         <v>2</v>
       </c>
-      <c r="F62"/>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
@@ -4788,7 +5510,9 @@
       <c r="E63" s="1">
         <v>2</v>
       </c>
-      <c r="F63"/>
+      <c r="F63" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
@@ -4806,7 +5530,9 @@
       <c r="E64" s="1">
         <v>2</v>
       </c>
-      <c r="F64"/>
+      <c r="F64" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -4824,7 +5550,9 @@
       <c r="E65" s="1">
         <v>2</v>
       </c>
-      <c r="F65"/>
+      <c r="F65" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
@@ -4842,7 +5570,9 @@
       <c r="E66" s="1">
         <v>2</v>
       </c>
-      <c r="F66"/>
+      <c r="F66" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
@@ -4860,7 +5590,9 @@
       <c r="E67" s="1">
         <v>2</v>
       </c>
-      <c r="F67"/>
+      <c r="F67" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
@@ -4878,7 +5610,9 @@
       <c r="E68" s="1">
         <v>2</v>
       </c>
-      <c r="F68"/>
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -4896,7 +5630,9 @@
       <c r="E69" s="1">
         <v>2</v>
       </c>
-      <c r="F69"/>
+      <c r="F69" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
@@ -4914,7 +5650,9 @@
       <c r="E70" s="1">
         <v>2</v>
       </c>
-      <c r="F70"/>
+      <c r="F70" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
@@ -4932,7 +5670,9 @@
       <c r="E71" s="1">
         <v>2</v>
       </c>
-      <c r="F71"/>
+      <c r="F71" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
@@ -4950,7 +5690,9 @@
       <c r="E72" s="1">
         <v>2</v>
       </c>
-      <c r="F72"/>
+      <c r="F72" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
@@ -4968,7 +5710,9 @@
       <c r="E73" s="1">
         <v>2</v>
       </c>
-      <c r="F73"/>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
@@ -4986,7 +5730,9 @@
       <c r="E74" s="1">
         <v>2</v>
       </c>
-      <c r="F74"/>
+      <c r="F74" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
@@ -5004,7 +5750,9 @@
       <c r="E75" s="1">
         <v>2</v>
       </c>
-      <c r="F75"/>
+      <c r="F75" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
@@ -5022,7 +5770,9 @@
       <c r="E76" s="1">
         <v>2</v>
       </c>
-      <c r="F76"/>
+      <c r="F76" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
@@ -5040,7 +5790,9 @@
       <c r="E77" s="1">
         <v>2</v>
       </c>
-      <c r="F77"/>
+      <c r="F77" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
@@ -5058,7 +5810,9 @@
       <c r="E78" s="1">
         <v>2</v>
       </c>
-      <c r="F78"/>
+      <c r="F78" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
@@ -5076,7 +5830,9 @@
       <c r="E79" s="1">
         <v>2</v>
       </c>
-      <c r="F79"/>
+      <c r="F79" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
@@ -5094,7 +5850,9 @@
       <c r="E80" s="1">
         <v>2</v>
       </c>
-      <c r="F80"/>
+      <c r="F80" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
@@ -5112,7 +5870,9 @@
       <c r="E81" s="1">
         <v>2</v>
       </c>
-      <c r="F81"/>
+      <c r="F81" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
@@ -5130,7 +5890,9 @@
       <c r="E82" s="1">
         <v>2</v>
       </c>
-      <c r="F82"/>
+      <c r="F82" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
@@ -5148,7 +5910,9 @@
       <c r="E83" s="1">
         <v>1</v>
       </c>
-      <c r="F83"/>
+      <c r="F83" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
@@ -5166,7 +5930,9 @@
       <c r="E84" s="1">
         <v>1</v>
       </c>
-      <c r="F84"/>
+      <c r="F84" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
@@ -5184,7 +5950,9 @@
       <c r="E85" s="1">
         <v>1</v>
       </c>
-      <c r="F85"/>
+      <c r="F85" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
@@ -5202,7 +5970,9 @@
       <c r="E86" s="1">
         <v>1</v>
       </c>
-      <c r="F86"/>
+      <c r="F86" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
@@ -5220,7 +5990,9 @@
       <c r="E87" s="1">
         <v>1</v>
       </c>
-      <c r="F87"/>
+      <c r="F87" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
@@ -5238,7 +6010,9 @@
       <c r="E88" s="1">
         <v>1</v>
       </c>
-      <c r="F88"/>
+      <c r="F88" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
@@ -5256,7 +6030,9 @@
       <c r="E89" s="1">
         <v>1</v>
       </c>
-      <c r="F89"/>
+      <c r="F89" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
@@ -5274,7 +6050,9 @@
       <c r="E90" s="1">
         <v>1</v>
       </c>
-      <c r="F90"/>
+      <c r="F90" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
@@ -5292,7 +6070,9 @@
       <c r="E91" s="1">
         <v>1</v>
       </c>
-      <c r="F91"/>
+      <c r="F91" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
@@ -5310,7 +6090,9 @@
       <c r="E92" s="1">
         <v>1</v>
       </c>
-      <c r="F92"/>
+      <c r="F92" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
@@ -5328,7 +6110,9 @@
       <c r="E93" s="1">
         <v>0</v>
       </c>
-      <c r="F93"/>
+      <c r="F93" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
@@ -5346,7 +6130,9 @@
       <c r="E94" s="1">
         <v>0</v>
       </c>
-      <c r="F94"/>
+      <c r="F94" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
@@ -5364,7 +6150,9 @@
       <c r="E95" s="1">
         <v>0</v>
       </c>
-      <c r="F95"/>
+      <c r="F95" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
@@ -5382,7 +6170,9 @@
       <c r="E96" s="1">
         <v>0</v>
       </c>
-      <c r="F96"/>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
@@ -5400,7 +6190,9 @@
       <c r="E97" s="1">
         <v>0</v>
       </c>
-      <c r="F97"/>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
@@ -5418,7 +6210,9 @@
       <c r="E98" s="1">
         <v>0</v>
       </c>
-      <c r="F98"/>
+      <c r="F98" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
@@ -5436,7 +6230,9 @@
       <c r="E99" s="1">
         <v>0</v>
       </c>
-      <c r="F99"/>
+      <c r="F99" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
@@ -5454,7 +6250,9 @@
       <c r="E100" s="1">
         <v>0</v>
       </c>
-      <c r="F100"/>
+      <c r="F100" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
@@ -5472,7 +6270,9 @@
       <c r="E101" s="1">
         <v>0</v>
       </c>
-      <c r="F101"/>
+      <c r="F101" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
@@ -5490,7 +6290,9 @@
       <c r="E102" s="1">
         <v>0</v>
       </c>
-      <c r="F102"/>
+      <c r="F102" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>